<commit_message>
small bugs fixed, images added
</commit_message>
<xml_diff>
--- a/stock_tracker.xlsx
+++ b/stock_tracker.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MyInvestments" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>aapl</t>
         </is>
@@ -474,29 +474,86 @@
         <v>226.9833984375</v>
       </c>
       <c r="D2" t="n">
-        <v>271.8399963378906</v>
+        <v>272.1900024414062</v>
       </c>
       <c r="E2" t="n">
         <v>20.98</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>goog</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1984</v>
+        <v>14296</v>
       </c>
       <c r="C3" t="n">
-        <v>218.8023100645767</v>
+        <v>204.2062094332519</v>
       </c>
       <c r="D3" t="n">
-        <v>298.0599975585938</v>
+        <v>303.75</v>
       </c>
       <c r="E3" t="n">
-        <v>43.37143520762952</v>
+        <v>50.69571676610289</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>amzn</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>129</v>
+      </c>
+      <c r="C4" t="n">
+        <v>237.4199981689453</v>
+      </c>
+      <c r="D4" t="n">
+        <v>226.7599945068359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-6.802288779815519</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>celh</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>120</v>
+      </c>
+      <c r="C5" t="n">
+        <v>23.76000022888184</v>
+      </c>
+      <c r="D5" t="n">
+        <v>41.66999816894531</v>
+      </c>
+      <c r="E5" t="n">
+        <v>71.8434403945129</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rivn</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>150</v>
+      </c>
+      <c r="C6" t="n">
+        <v>13.8100004196167</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20.28000068664551</v>
+      </c>
+      <c r="E6" t="n">
+        <v>46.8501091269944</v>
       </c>
     </row>
   </sheetData>
@@ -550,19 +607,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>714201.2968399951</v>
+        <v>3234979.363583846</v>
       </c>
       <c r="D2" t="n">
-        <v>3218</v>
+        <v>15929</v>
       </c>
       <c r="E2" t="n">
-        <v>221.9394955997499</v>
+        <v>203.0874106085659</v>
       </c>
       <c r="F2" t="n">
-        <v>27.84169232599559</v>
+        <v>22.44052187499769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review of code, small bugs fixed
</commit_message>
<xml_diff>
--- a/stock_tracker.xlsx
+++ b/stock_tracker.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,96 +464,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aapl</t>
+          <t>tsla</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1234</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>226.9833984375</v>
+        <v>397.2099914550781</v>
       </c>
       <c r="D2" t="n">
-        <v>272.1900024414062</v>
+        <v>417.0700073242188</v>
       </c>
       <c r="E2" t="n">
-        <v>20.98</v>
+        <v>5.093026716730011</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>goog</t>
+          <t>nmm</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14296</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>204.2062094332519</v>
+        <v>55.43999862670898</v>
       </c>
       <c r="D3" t="n">
-        <v>303.75</v>
+        <v>60.33000183105469</v>
       </c>
       <c r="E3" t="n">
-        <v>50.69571676610289</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>amzn</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>129</v>
-      </c>
-      <c r="C4" t="n">
-        <v>237.4199981689453</v>
-      </c>
-      <c r="D4" t="n">
-        <v>226.7599945068359</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-6.802288779815519</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>celh</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>120</v>
-      </c>
-      <c r="C5" t="n">
-        <v>23.76000022888184</v>
-      </c>
-      <c r="D5" t="n">
-        <v>41.66999816894531</v>
-      </c>
-      <c r="E5" t="n">
-        <v>71.8434403945129</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>rivn</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>150</v>
-      </c>
-      <c r="C6" t="n">
-        <v>13.8100004196167</v>
-      </c>
-      <c r="D6" t="n">
-        <v>20.28000068664551</v>
-      </c>
-      <c r="E6" t="n">
-        <v>46.8501091269944</v>
+        <v>11.72438701480872</v>
       </c>
     </row>
   </sheetData>
@@ -607,19 +550,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3234979.363583846</v>
+        <v>6817.79984664917</v>
       </c>
       <c r="D2" t="n">
-        <v>15929</v>
+        <v>49</v>
       </c>
       <c r="E2" t="n">
-        <v>203.0874106085659</v>
+        <v>139.1387723805953</v>
       </c>
       <c r="F2" t="n">
-        <v>22.44052187499769</v>
+        <v>5.46780506258587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>